<commit_message>
Finished offline excel integration
Need to add writing to excel files and accessing online excel files
</commit_message>
<xml_diff>
--- a/WFSC_DATA (3).xlsx
+++ b/WFSC_DATA (3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\GitHub\test-sailing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77157709-D363-456D-BD22-62266F872B43}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9B9F58-B276-456C-8E02-B02918DEB49C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" tabRatio="782" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" tabRatio="782" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="25" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">MROA!$A$3:$D$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Results (handicap)'!$B$1:$J$102</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Results (Pursuit)'!$A$2:$M$2</definedName>
-    <definedName name="_xlcn.WorksheetConnection_wfscSailorsAE1" hidden="1">wfscSailors!$A:$E</definedName>
+    <definedName name="_xlcn.WorksheetConnection_wfscSailorsAE" hidden="1">wfscSailors!$A:$E</definedName>
     <definedName name="Ashton_Keynes" localSheetId="5">#REF!</definedName>
     <definedName name="Ashton_Keynes">#REF!</definedName>
     <definedName name="MROA">MROA!$A$1:$D$22</definedName>
@@ -78,7 +78,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_wfscSailorsAE1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_wfscSailorsAE"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3031" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3032" uniqueCount="647">
   <si>
     <t>Row Labels</t>
   </si>
@@ -2026,6 +2026,9 @@
   </si>
   <si>
     <t>Windermere Cruising Association</t>
+  </si>
+  <si>
+    <t>Q ba</t>
   </si>
 </sst>
 </file>
@@ -7209,273 +7212,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1AD6032F-D292-4B02-9925-A89E3A76BE74}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="48">
-        <item x="46"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0">
-      <items count="36">
-        <item x="22"/>
-        <item x="12"/>
-        <item x="32"/>
-        <item x="30"/>
-        <item x="18"/>
-        <item x="21"/>
-        <item x="28"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="8"/>
-        <item x="27"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="24"/>
-        <item x="17"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="14"/>
-        <item x="23"/>
-        <item x="19"/>
-        <item x="11"/>
-        <item x="29"/>
-        <item x="33"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item x="25"/>
-        <item x="16"/>
-        <item x="26"/>
-        <item x="10"/>
-        <item x="15"/>
-        <item x="9"/>
-        <item x="31"/>
-        <item x="20"/>
-        <item x="5"/>
-        <item x="34"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="48">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Class" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE789B38-1E1D-4EB9-9DBB-F7D968D4FD47}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:E51" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
@@ -7738,6 +7474,273 @@
   <dataFields count="2">
     <dataField name="Count of Class" fld="2" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Sum of SailNo" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1AD6032F-D292-4B02-9925-A89E3A76BE74}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="48">
+        <item x="46"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="36">
+        <item x="22"/>
+        <item x="12"/>
+        <item x="32"/>
+        <item x="30"/>
+        <item x="18"/>
+        <item x="21"/>
+        <item x="28"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="8"/>
+        <item x="27"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="24"/>
+        <item x="17"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="14"/>
+        <item x="23"/>
+        <item x="19"/>
+        <item x="11"/>
+        <item x="29"/>
+        <item x="33"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="25"/>
+        <item x="16"/>
+        <item x="26"/>
+        <item x="10"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="31"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="34"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="48">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Class" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -10366,7 +10369,7 @@
   </sheetPr>
   <dimension ref="A1:M164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A134" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -19538,8 +19541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W202"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21150,16 +21153,18 @@
       <c r="A57" s="121" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="140"/>
+      <c r="B57" s="140">
+        <v>123456</v>
+      </c>
       <c r="C57" s="104" t="s">
-        <v>92</v>
+        <v>646</v>
       </c>
       <c r="D57" s="105" t="s">
         <v>64</v>
       </c>
       <c r="E57" s="108" t="str">
         <f>Table1[[#This Row],[HelmName]] &amp; " : " &amp; Table1[[#This Row],[Class]]</f>
-        <v>Wolly Merchant : Q'ba</v>
+        <v>Wolly Merchant : Q ba</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
@@ -21167,13 +21172,17 @@
       </c>
     </row>
     <row r="58" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="121"/>
-      <c r="B58" s="122"/>
+      <c r="A58" s="121" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="122">
+        <v>0</v>
+      </c>
       <c r="C58" s="122"/>
       <c r="D58" s="123"/>
       <c r="E58" s="141" t="str">
         <f>Table1[[#This Row],[HelmName]] &amp; " : " &amp; Table1[[#This Row],[Class]]</f>
-        <v xml:space="preserve"> : </v>
+        <v xml:space="preserve">- : </v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
@@ -21184,7 +21193,9 @@
       <c r="A59" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="122"/>
+      <c r="B59" s="122">
+        <v>0</v>
+      </c>
       <c r="C59" s="122"/>
       <c r="D59" s="123"/>
       <c r="E59" s="141" t="str">
@@ -21200,7 +21211,9 @@
       <c r="A60" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="104"/>
+      <c r="B60" s="104">
+        <v>0</v>
+      </c>
       <c r="C60" s="104"/>
       <c r="D60" s="123"/>
       <c r="E60" s="141" t="str">
@@ -21216,7 +21229,9 @@
       <c r="A61" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="104"/>
+      <c r="B61" s="104">
+        <v>0</v>
+      </c>
       <c r="C61" s="104"/>
       <c r="D61" s="123"/>
       <c r="E61" s="141" t="str">
@@ -21232,7 +21247,9 @@
       <c r="A62" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B62" s="104"/>
+      <c r="B62" s="104">
+        <v>0</v>
+      </c>
       <c r="C62" s="104"/>
       <c r="D62" s="123"/>
       <c r="E62" s="141" t="str">
@@ -21248,7 +21265,9 @@
       <c r="A63" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="104"/>
+      <c r="B63" s="104">
+        <v>0</v>
+      </c>
       <c r="C63" s="104"/>
       <c r="D63" s="123"/>
       <c r="E63" s="141" t="str">
@@ -21264,7 +21283,9 @@
       <c r="A64" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="104"/>
+      <c r="B64" s="104">
+        <v>0</v>
+      </c>
       <c r="C64" s="104"/>
       <c r="D64" s="123"/>
       <c r="E64" s="141" t="str">

</xml_diff>

<commit_message>
Changes data file slightly
</commit_message>
<xml_diff>
--- a/WFSC_DATA (3).xlsx
+++ b/WFSC_DATA (3).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luke\Documents\GitHub\test-sailing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77157709-D363-456D-BD22-62266F872B43}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C9B9F58-B276-456C-8E02-B02918DEB49C}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" tabRatio="782" firstSheet="2" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7650" tabRatio="782" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="25" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">MROA!$A$3:$D$21</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Results (handicap)'!$B$1:$J$102</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Results (Pursuit)'!$A$2:$M$2</definedName>
-    <definedName name="_xlcn.WorksheetConnection_wfscSailorsAE1" hidden="1">wfscSailors!$A:$E</definedName>
+    <definedName name="_xlcn.WorksheetConnection_wfscSailorsAE" hidden="1">wfscSailors!$A:$E</definedName>
     <definedName name="Ashton_Keynes" localSheetId="5">#REF!</definedName>
     <definedName name="Ashton_Keynes">#REF!</definedName>
     <definedName name="MROA">MROA!$A$1:$D$22</definedName>
@@ -78,7 +78,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="Range" autoDelete="1">
-          <x15:rangePr sourceName="_xlcn.WorksheetConnection_wfscSailorsAE1"/>
+          <x15:rangePr sourceName="_xlcn.WorksheetConnection_wfscSailorsAE"/>
         </x15:connection>
       </ext>
     </extLst>
@@ -87,7 +87,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3031" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3032" uniqueCount="647">
   <si>
     <t>Row Labels</t>
   </si>
@@ -2026,6 +2026,9 @@
   </si>
   <si>
     <t>Windermere Cruising Association</t>
+  </si>
+  <si>
+    <t>Q ba</t>
   </si>
 </sst>
 </file>
@@ -7209,273 +7212,6 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1AD6032F-D292-4B02-9925-A89E3A76BE74}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="A3:B51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="5">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="48">
-        <item x="46"/>
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item x="16"/>
-        <item x="17"/>
-        <item x="18"/>
-        <item x="19"/>
-        <item x="20"/>
-        <item x="21"/>
-        <item x="22"/>
-        <item x="23"/>
-        <item x="24"/>
-        <item x="25"/>
-        <item x="26"/>
-        <item x="27"/>
-        <item x="28"/>
-        <item x="29"/>
-        <item x="30"/>
-        <item x="31"/>
-        <item x="32"/>
-        <item x="33"/>
-        <item x="34"/>
-        <item x="35"/>
-        <item x="36"/>
-        <item x="37"/>
-        <item x="38"/>
-        <item x="39"/>
-        <item x="40"/>
-        <item x="41"/>
-        <item x="42"/>
-        <item x="43"/>
-        <item x="44"/>
-        <item x="45"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0">
-      <items count="36">
-        <item x="22"/>
-        <item x="12"/>
-        <item x="32"/>
-        <item x="30"/>
-        <item x="18"/>
-        <item x="21"/>
-        <item x="28"/>
-        <item x="0"/>
-        <item x="13"/>
-        <item x="8"/>
-        <item x="27"/>
-        <item x="4"/>
-        <item x="6"/>
-        <item x="24"/>
-        <item x="17"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="14"/>
-        <item x="23"/>
-        <item x="19"/>
-        <item x="11"/>
-        <item x="29"/>
-        <item x="33"/>
-        <item x="1"/>
-        <item x="7"/>
-        <item x="25"/>
-        <item x="16"/>
-        <item x="26"/>
-        <item x="10"/>
-        <item x="15"/>
-        <item x="9"/>
-        <item x="31"/>
-        <item x="20"/>
-        <item x="5"/>
-        <item x="34"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="48">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i>
-      <x v="16"/>
-    </i>
-    <i>
-      <x v="17"/>
-    </i>
-    <i>
-      <x v="18"/>
-    </i>
-    <i>
-      <x v="19"/>
-    </i>
-    <i>
-      <x v="20"/>
-    </i>
-    <i>
-      <x v="21"/>
-    </i>
-    <i>
-      <x v="22"/>
-    </i>
-    <i>
-      <x v="23"/>
-    </i>
-    <i>
-      <x v="24"/>
-    </i>
-    <i>
-      <x v="25"/>
-    </i>
-    <i>
-      <x v="26"/>
-    </i>
-    <i>
-      <x v="27"/>
-    </i>
-    <i>
-      <x v="28"/>
-    </i>
-    <i>
-      <x v="29"/>
-    </i>
-    <i>
-      <x v="30"/>
-    </i>
-    <i>
-      <x v="31"/>
-    </i>
-    <i>
-      <x v="32"/>
-    </i>
-    <i>
-      <x v="33"/>
-    </i>
-    <i>
-      <x v="34"/>
-    </i>
-    <i>
-      <x v="35"/>
-    </i>
-    <i>
-      <x v="36"/>
-    </i>
-    <i>
-      <x v="37"/>
-    </i>
-    <i>
-      <x v="38"/>
-    </i>
-    <i>
-      <x v="39"/>
-    </i>
-    <i>
-      <x v="40"/>
-    </i>
-    <i>
-      <x v="41"/>
-    </i>
-    <i>
-      <x v="42"/>
-    </i>
-    <i>
-      <x v="43"/>
-    </i>
-    <i>
-      <x v="44"/>
-    </i>
-    <i>
-      <x v="45"/>
-    </i>
-    <i>
-      <x v="46"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Count of Class" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DE789B38-1E1D-4EB9-9DBB-F7D968D4FD47}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:E51" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="5">
@@ -7738,6 +7474,273 @@
   <dataFields count="2">
     <dataField name="Count of Class" fld="2" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Sum of SailNo" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1AD6032F-D292-4B02-9925-A89E3A76BE74}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="5">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="48">
+        <item x="46"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item x="16"/>
+        <item x="17"/>
+        <item x="18"/>
+        <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="40"/>
+        <item x="41"/>
+        <item x="42"/>
+        <item x="43"/>
+        <item x="44"/>
+        <item x="45"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0">
+      <items count="36">
+        <item x="22"/>
+        <item x="12"/>
+        <item x="32"/>
+        <item x="30"/>
+        <item x="18"/>
+        <item x="21"/>
+        <item x="28"/>
+        <item x="0"/>
+        <item x="13"/>
+        <item x="8"/>
+        <item x="27"/>
+        <item x="4"/>
+        <item x="6"/>
+        <item x="24"/>
+        <item x="17"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="14"/>
+        <item x="23"/>
+        <item x="19"/>
+        <item x="11"/>
+        <item x="29"/>
+        <item x="33"/>
+        <item x="1"/>
+        <item x="7"/>
+        <item x="25"/>
+        <item x="16"/>
+        <item x="26"/>
+        <item x="10"/>
+        <item x="15"/>
+        <item x="9"/>
+        <item x="31"/>
+        <item x="20"/>
+        <item x="5"/>
+        <item x="34"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="48">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Class" fld="2" subtotal="count" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -10366,7 +10369,7 @@
   </sheetPr>
   <dimension ref="A1:M164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A134" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A134" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
@@ -19538,8 +19541,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W202"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21150,16 +21153,18 @@
       <c r="A57" s="121" t="s">
         <v>48</v>
       </c>
-      <c r="B57" s="140"/>
+      <c r="B57" s="140">
+        <v>123456</v>
+      </c>
       <c r="C57" s="104" t="s">
-        <v>92</v>
+        <v>646</v>
       </c>
       <c r="D57" s="105" t="s">
         <v>64</v>
       </c>
       <c r="E57" s="108" t="str">
         <f>Table1[[#This Row],[HelmName]] &amp; " : " &amp; Table1[[#This Row],[Class]]</f>
-        <v>Wolly Merchant : Q'ba</v>
+        <v>Wolly Merchant : Q ba</v>
       </c>
       <c r="H57" t="str">
         <f t="shared" si="0"/>
@@ -21167,13 +21172,17 @@
       </c>
     </row>
     <row r="58" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="121"/>
-      <c r="B58" s="122"/>
+      <c r="A58" s="121" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="122">
+        <v>0</v>
+      </c>
       <c r="C58" s="122"/>
       <c r="D58" s="123"/>
       <c r="E58" s="141" t="str">
         <f>Table1[[#This Row],[HelmName]] &amp; " : " &amp; Table1[[#This Row],[Class]]</f>
-        <v xml:space="preserve"> : </v>
+        <v xml:space="preserve">- : </v>
       </c>
       <c r="H58" t="str">
         <f t="shared" si="0"/>
@@ -21184,7 +21193,9 @@
       <c r="A59" s="121" t="s">
         <v>3</v>
       </c>
-      <c r="B59" s="122"/>
+      <c r="B59" s="122">
+        <v>0</v>
+      </c>
       <c r="C59" s="122"/>
       <c r="D59" s="123"/>
       <c r="E59" s="141" t="str">
@@ -21200,7 +21211,9 @@
       <c r="A60" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B60" s="104"/>
+      <c r="B60" s="104">
+        <v>0</v>
+      </c>
       <c r="C60" s="104"/>
       <c r="D60" s="123"/>
       <c r="E60" s="141" t="str">
@@ -21216,7 +21229,9 @@
       <c r="A61" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B61" s="104"/>
+      <c r="B61" s="104">
+        <v>0</v>
+      </c>
       <c r="C61" s="104"/>
       <c r="D61" s="123"/>
       <c r="E61" s="141" t="str">
@@ -21232,7 +21247,9 @@
       <c r="A62" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B62" s="104"/>
+      <c r="B62" s="104">
+        <v>0</v>
+      </c>
       <c r="C62" s="104"/>
       <c r="D62" s="123"/>
       <c r="E62" s="141" t="str">
@@ -21248,7 +21265,9 @@
       <c r="A63" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B63" s="104"/>
+      <c r="B63" s="104">
+        <v>0</v>
+      </c>
       <c r="C63" s="104"/>
       <c r="D63" s="123"/>
       <c r="E63" s="141" t="str">
@@ -21264,7 +21283,9 @@
       <c r="A64" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="B64" s="104"/>
+      <c r="B64" s="104">
+        <v>0</v>
+      </c>
       <c r="C64" s="104"/>
       <c r="D64" s="123"/>
       <c r="E64" s="141" t="str">

</xml_diff>